<commit_message>
Integration of Na's work
</commit_message>
<xml_diff>
--- a/New Reports/Team05Report.xlsx
+++ b/New Reports/Team05Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Code\Python\2019fall-Group5-555B-Project\New Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vctu\OneDrive\Code\Python\2019fall-Group5-555B-Project\New Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_91594EE21CD72D0513AB51B7F1FA2014BFDA855E" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B3E0665B-F8BA-4E9F-8A3B-144B40E44E0A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{9FF38008-5B28-4D0E-8EBD-1572661F0983}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1310" yWindow="3570" windowWidth="28800" windowHeight="15460" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -2032,15 +2032,15 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.453125" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" customWidth="1"/>
-    <col min="4" max="5" width="20.453125" customWidth="1"/>
+    <col min="1" max="1" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.4609375" customWidth="1"/>
+    <col min="3" max="3" width="8.4609375" customWidth="1"/>
+    <col min="4" max="5" width="20.4609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D9" s="4" t="s">
         <v>50</v>
       </c>
@@ -2134,16 +2134,16 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" customWidth="1"/>
-    <col min="2" max="2" width="7.6328125" customWidth="1"/>
-    <col min="3" max="3" width="19.453125" customWidth="1"/>
-    <col min="4" max="4" width="6.6328125" customWidth="1"/>
-    <col min="5" max="5" width="7.6328125" customWidth="1"/>
+    <col min="1" max="1" width="5.15234375" customWidth="1"/>
+    <col min="2" max="2" width="7.61328125" customWidth="1"/>
+    <col min="3" max="3" width="19.4609375" customWidth="1"/>
+    <col min="4" max="4" width="6.61328125" customWidth="1"/>
+    <col min="5" max="5" width="7.61328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>41</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2223,47 +2223,47 @@
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="7"/>
-    <col min="2" max="2" width="9.453125" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.84375" style="7"/>
+    <col min="2" max="2" width="9.4609375" customWidth="1"/>
+    <col min="3" max="3" width="15.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.3828125" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" customWidth="1"/>
+    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>182</v>
       </c>
@@ -2286,7 +2286,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>183</v>
       </c>
@@ -2302,7 +2302,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>184</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>185</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>186</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>187</v>
       </c>
@@ -2418,17 +2418,17 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="2"/>
-    <col min="2" max="2" width="16.6328125" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" customWidth="1"/>
-    <col min="4" max="4" width="7.1796875" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.84375" style="2"/>
+    <col min="2" max="2" width="16.61328125" customWidth="1"/>
+    <col min="3" max="3" width="12.4609375" customWidth="1"/>
+    <col min="4" max="4" width="7.15234375" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" customWidth="1"/>
+    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2448,7 +2448,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>40442</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>40455</v>
       </c>
@@ -2497,19 +2497,19 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.6328125" customWidth="1"/>
-    <col min="2" max="2" width="24.54296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6328125" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" customWidth="1"/>
-    <col min="6" max="6" width="7.453125" customWidth="1"/>
-    <col min="7" max="7" width="6.6328125" customWidth="1"/>
-    <col min="8" max="8" width="7.6328125" customWidth="1"/>
-    <col min="9" max="9" width="10.81640625" style="6"/>
+    <col min="1" max="1" width="7.61328125" customWidth="1"/>
+    <col min="2" max="2" width="24.53515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.61328125" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" customWidth="1"/>
+    <col min="6" max="6" width="7.4609375" customWidth="1"/>
+    <col min="7" max="7" width="6.61328125" customWidth="1"/>
+    <col min="8" max="8" width="7.61328125" customWidth="1"/>
+    <col min="9" max="9" width="10.84375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -2549,7 +2549,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>135</v>
       </c>
@@ -2560,7 +2560,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>136</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>137</v>
       </c>
@@ -2582,7 +2582,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>138</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>139</v>
       </c>
@@ -2604,7 +2604,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>140</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>141</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>142</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>143</v>
       </c>
@@ -2648,36 +2648,36 @@
         <v>201</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" s="5"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2" ht="27" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>52</v>
       </c>
@@ -2697,9 +2697,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2743,9 +2743,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2788,9 +2788,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2833,13 +2833,13 @@
       <selection activeCell="A11" sqref="A10:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.15234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.4609375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>133</v>
       </c>
@@ -2850,7 +2850,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>135</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>136</v>
       </c>
@@ -2883,7 +2883,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>137</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>138</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>139</v>
       </c>
@@ -2916,7 +2916,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>140</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>141</v>
       </c>
@@ -2938,7 +2938,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>142</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>143</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>144</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>145</v>
       </c>
@@ -2982,7 +2982,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>146</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>147</v>
       </c>
@@ -3004,7 +3004,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>148</v>
       </c>
@@ -3015,7 +3015,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>149</v>
       </c>
@@ -3026,7 +3026,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>150</v>
       </c>
@@ -3037,7 +3037,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>151</v>
       </c>
@@ -3048,7 +3048,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>152</v>
       </c>
@@ -3059,7 +3059,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>153</v>
       </c>
@@ -3070,7 +3070,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>154</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>155</v>
       </c>
@@ -3092,7 +3092,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>156</v>
       </c>
@@ -3103,7 +3103,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>157</v>
       </c>
@@ -3114,7 +3114,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>158</v>
       </c>
@@ -3125,7 +3125,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>159</v>
       </c>
@@ -3136,7 +3136,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>160</v>
       </c>
@@ -3147,7 +3147,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>161</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>162</v>
       </c>
@@ -3169,7 +3169,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>163</v>
       </c>
@@ -3180,7 +3180,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>164</v>
       </c>
@@ -3191,7 +3191,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>165</v>
       </c>
@@ -3202,7 +3202,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>166</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>167</v>
       </c>
@@ -3224,7 +3224,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>168</v>
       </c>
@@ -3235,7 +3235,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>169</v>
       </c>
@@ -3246,7 +3246,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>170</v>
       </c>
@@ -3257,7 +3257,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>171</v>
       </c>
@@ -3268,7 +3268,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>172</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>173</v>
       </c>
@@ -3290,7 +3290,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>174</v>
       </c>
@@ -3301,7 +3301,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>175</v>
       </c>

</xml_diff>